<commit_message>
enable to use mandatory option on two poiji annotations
Signed-off-by: Hakan Ozler <ozler.hakan@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/hidden.xlsx
+++ b/src/test/resources/hidden.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\NetBeansProjects\poiji\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakan/IdeaProjects/p2o/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B782CCB-2DC4-AF4A-A792-0C29DB58C450}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="0" windowWidth="19500" windowHeight="8115" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="19500" windowHeight="8120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hidden 1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -89,12 +90,15 @@
   </si>
   <si>
     <t>HIDDEN 2</t>
+  </si>
+  <si>
+    <t>Insurance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,16 +454,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -470,16 +474,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E1" sqref="E1:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,8 +496,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -506,8 +513,11 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -520,8 +530,11 @@
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -534,8 +547,11 @@
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -548,8 +564,11 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -562,30 +581,33 @@
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E6">
+        <v>-12</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>

</xml_diff>